<commit_message>
[LSK]Rabbie Furniture And Facilities-Basic 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/[LSK]Rabbie Furniture And Facilities-Basic - 3155273482/3155273482.xlsx
+++ b/Data/[LSK]Rabbie Furniture And Facilities-Basic - 3155273482/3155273482.xlsx
@@ -5,15 +5,16 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\[LSK]Rabbie Furniture And Facilities-Basic - 3155273482\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\[LSK]Rabbie Furniture And Facilities-Basic - 3155273482\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CEB308-8E81-4265-8D01-A01462D00330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B6D647-EF31-46F8-BD08-6D503E559DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240213" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="616">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1772,13 +1795,393 @@
   <si>
     <t>달의 목재</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플라네타리움을 추출하는 중.</t>
+  </si>
+  <si>
+    <t>달의 합금을 생산하기 위해 사용 가능한 재료를 활용합니다. 전문 장비를 사용하는 것만큼 속도와 양이 효율적이지는 않지만, 상세한 제련 공정과 적절한 장비로 인해 품질은 여전히 ​​보장됩니다.</t>
+  </si>
+  <si>
+    <t>달의 합금 제작 중.</t>
+  </si>
+  <si>
+    <t>일반적인 소파보다 두배 더 커다랗고 푹신푹신한 소파입니다. 구름 위에 앉아있는 느낌을 받을 수 있습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_SHS_Meal_Sideboard.label</t>
+  </si>
+  <si>
+    <t>음식 선반</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_SHS_Meal_Sideboard.description</t>
+  </si>
+  <si>
+    <t>장식용 음식 선반입니다. 안에 뭐가 있는지 볼까요... 여기도 당근, 저기도 당근, 온통 당근이군요. 흠.</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_RB_Item_Shelf.label</t>
+  </si>
+  <si>
+    <t>선반</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_RB_Item_Shelf.description</t>
+  </si>
+  <si>
+    <t>달의 도시 창고에서 볼 수 있는 선반입니다. 맨 위쪽은 아무래도 평범한 래비들에겐 조금 높은 것 같습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_SHS_Bookshelf.label</t>
+  </si>
+  <si>
+    <t>책장</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_SHS_Bookshelf.description</t>
+  </si>
+  <si>
+    <t>여러 가지 종류의 책이 꽂혀 있는 책장입니다, 자기 전에 읽기 좋습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_SHS_Bookshelf_empty.label</t>
+  </si>
+  <si>
+    <t>책장(비어 있음)</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_SHS_Bookshelf_empty.description</t>
+  </si>
+  <si>
+    <t>텅 비어있는 책장입니다. 가끔은 비워두는 것도 나쁘지 않죠.</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_SHS_Mirror.label</t>
+  </si>
+  <si>
+    <t>거울</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_SHS_Mirror.description</t>
+  </si>
+  <si>
+    <t>래비들이 옷을 갈아입을 때 사용하는 거울입니다.\n\n이데올로기 DLC가 있다면, 이 곳에서 외형을 바꿀 수 있습니다.</t>
+  </si>
+  <si>
+    <t>{0}을 먹는 중.</t>
+  </si>
+  <si>
+    <t>ThingDef+LSK_Board.tools.log.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>장식용</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>음식</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선반입니다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>안에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뭐가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있는지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>볼까요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">... </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>여기도</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>홍당무</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>저기도</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>홍당무</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>온통</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>홍당무 뿐이군요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>흠</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LSK_SHS_Meal_Sideboard.label</t>
+  </si>
+  <si>
+    <t>LSK_SHS_Meal_Sideboard.description</t>
+  </si>
+  <si>
+    <t>LSK_RB_Item_Shelf.label</t>
+  </si>
+  <si>
+    <t>LSK_RB_Item_Shelf.description</t>
+  </si>
+  <si>
+    <t>LSK_SHS_Bookshelf.label</t>
+  </si>
+  <si>
+    <t>LSK_SHS_Bookshelf.description</t>
+  </si>
+  <si>
+    <t>LSK_SHS_Bookshelf_empty.label</t>
+  </si>
+  <si>
+    <t>LSK_SHS_Bookshelf_empty.description</t>
+  </si>
+  <si>
+    <t>LSK_SHS_Mirror.label</t>
+  </si>
+  <si>
+    <t>LSK_SHS_Mirror.description</t>
+  </si>
+  <si>
+    <t>LSK_Board.tools.log.label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1794,6 +2197,27 @@
     <font>
       <sz val="8"/>
       <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
@@ -1818,9 +2242,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2123,24 +2553,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EB21F7-3ADC-4DF4-96DD-663D253657AB}">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="72.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="72.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2160,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2177,7 +2607,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2194,7 +2624,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -2211,7 +2641,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2228,7 +2658,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -2245,7 +2675,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -2262,7 +2692,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2279,7 +2709,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -2296,7 +2726,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -2313,7 +2743,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -2330,7 +2760,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -2347,7 +2777,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -2364,7 +2794,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -2381,7 +2811,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -2398,7 +2828,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -2415,7 +2845,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2432,7 +2862,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
@@ -2449,7 +2879,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>56</v>
       </c>
@@ -2466,7 +2896,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
@@ -2483,7 +2913,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -2500,7 +2930,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
@@ -2517,7 +2947,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
@@ -2534,7 +2964,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -2551,7 +2981,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -2568,7 +2998,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
@@ -2585,7 +3015,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
@@ -2602,7 +3032,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -2619,7 +3049,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
@@ -2636,7 +3066,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>84</v>
       </c>
@@ -2653,7 +3083,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
@@ -2670,7 +3100,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
         <v>90</v>
       </c>
@@ -2687,7 +3117,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>93</v>
       </c>
@@ -2704,7 +3134,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
         <v>97</v>
       </c>
@@ -2721,7 +3151,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>100</v>
       </c>
@@ -2738,7 +3168,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
         <v>103</v>
       </c>
@@ -2755,7 +3185,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>106</v>
       </c>
@@ -2772,7 +3202,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
         <v>110</v>
       </c>
@@ -2789,7 +3219,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
@@ -2806,7 +3236,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
         <v>116</v>
       </c>
@@ -2823,7 +3253,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
         <v>119</v>
       </c>
@@ -2840,7 +3270,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
         <v>122</v>
       </c>
@@ -2857,7 +3287,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
         <v>125</v>
       </c>
@@ -2874,7 +3304,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
         <v>128</v>
       </c>
@@ -2891,7 +3321,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
         <v>131</v>
       </c>
@@ -2908,7 +3338,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
         <v>134</v>
       </c>
@@ -2925,7 +3355,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
         <v>137</v>
       </c>
@@ -2942,7 +3372,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
         <v>140</v>
       </c>
@@ -2959,7 +3389,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
         <v>143</v>
       </c>
@@ -2976,7 +3406,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
         <v>146</v>
       </c>
@@ -2993,7 +3423,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
         <v>148</v>
       </c>
@@ -3010,7 +3440,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
         <v>151</v>
       </c>
@@ -3027,7 +3457,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6">
       <c r="A53" s="1" t="s">
         <v>154</v>
       </c>
@@ -3044,7 +3474,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
         <v>157</v>
       </c>
@@ -3061,7 +3491,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
         <v>159</v>
       </c>
@@ -3078,7 +3508,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
         <v>162</v>
       </c>
@@ -3095,7 +3525,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
         <v>165</v>
       </c>
@@ -3112,7 +3542,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6">
       <c r="A58" s="1" t="s">
         <v>168</v>
       </c>
@@ -3129,7 +3559,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6">
       <c r="A59" s="1" t="s">
         <v>171</v>
       </c>
@@ -3146,7 +3576,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6">
       <c r="A60" s="1" t="s">
         <v>174</v>
       </c>
@@ -3163,7 +3593,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6">
       <c r="A61" s="1" t="s">
         <v>177</v>
       </c>
@@ -3180,7 +3610,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6">
       <c r="A62" s="1" t="s">
         <v>180</v>
       </c>
@@ -3197,7 +3627,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6">
       <c r="A63" s="1" t="s">
         <v>183</v>
       </c>
@@ -3214,7 +3644,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6">
       <c r="A64" s="1" t="s">
         <v>186</v>
       </c>
@@ -3231,7 +3661,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6">
       <c r="A65" s="1" t="s">
         <v>189</v>
       </c>
@@ -3248,7 +3678,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6">
       <c r="A66" s="1" t="s">
         <v>192</v>
       </c>
@@ -3265,7 +3695,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6">
       <c r="A67" s="1" t="s">
         <v>194</v>
       </c>
@@ -3282,7 +3712,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6">
       <c r="A68" s="1" t="s">
         <v>197</v>
       </c>
@@ -3299,7 +3729,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6">
       <c r="A69" s="1" t="s">
         <v>200</v>
       </c>
@@ -3316,7 +3746,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6">
       <c r="A70" s="1" t="s">
         <v>203</v>
       </c>
@@ -3333,7 +3763,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6">
       <c r="A71" s="1" t="s">
         <v>206</v>
       </c>
@@ -3350,7 +3780,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6">
       <c r="A72" s="1" t="s">
         <v>209</v>
       </c>
@@ -3367,7 +3797,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6">
       <c r="A73" s="1" t="s">
         <v>212</v>
       </c>
@@ -3384,7 +3814,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6">
       <c r="A74" s="1" t="s">
         <v>215</v>
       </c>
@@ -3401,7 +3831,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6">
       <c r="A75" s="1" t="s">
         <v>217</v>
       </c>
@@ -3418,7 +3848,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6">
       <c r="A76" s="1" t="s">
         <v>220</v>
       </c>
@@ -3435,7 +3865,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
         <v>222</v>
       </c>
@@ -3452,7 +3882,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6">
       <c r="A78" s="1" t="s">
         <v>225</v>
       </c>
@@ -3469,7 +3899,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
         <v>228</v>
       </c>
@@ -3486,7 +3916,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
         <v>231</v>
       </c>
@@ -3503,7 +3933,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6">
       <c r="A81" s="1" t="s">
         <v>234</v>
       </c>
@@ -3520,7 +3950,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6">
       <c r="A82" s="1" t="s">
         <v>237</v>
       </c>
@@ -3537,7 +3967,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6">
       <c r="A83" s="1" t="s">
         <v>240</v>
       </c>
@@ -3554,7 +3984,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6">
       <c r="A84" s="1" t="s">
         <v>243</v>
       </c>
@@ -3571,7 +4001,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6">
       <c r="A85" s="1" t="s">
         <v>246</v>
       </c>
@@ -3588,7 +4018,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6">
       <c r="A86" s="1" t="s">
         <v>249</v>
       </c>
@@ -3605,7 +4035,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
         <v>252</v>
       </c>
@@ -3622,7 +4052,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6">
       <c r="A88" s="1" t="s">
         <v>255</v>
       </c>
@@ -3639,7 +4069,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
         <v>258</v>
       </c>
@@ -3656,7 +4086,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
         <v>261</v>
       </c>
@@ -3673,7 +4103,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6">
       <c r="A91" s="1" t="s">
         <v>264</v>
       </c>
@@ -3690,7 +4120,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6">
       <c r="A92" s="1" t="s">
         <v>267</v>
       </c>
@@ -3707,7 +4137,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6">
       <c r="A93" s="1" t="s">
         <v>270</v>
       </c>
@@ -3724,7 +4154,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6">
       <c r="A94" s="1" t="s">
         <v>273</v>
       </c>
@@ -3741,7 +4171,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6">
       <c r="A95" s="1" t="s">
         <v>276</v>
       </c>
@@ -3758,7 +4188,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6">
       <c r="A96" s="1" t="s">
         <v>279</v>
       </c>
@@ -3775,7 +4205,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6">
       <c r="A97" s="1" t="s">
         <v>282</v>
       </c>
@@ -3792,7 +4222,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6">
       <c r="A98" s="1" t="s">
         <v>285</v>
       </c>
@@ -3809,7 +4239,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6">
       <c r="A99" s="1" t="s">
         <v>288</v>
       </c>
@@ -3826,7 +4256,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6">
       <c r="A100" s="1" t="s">
         <v>291</v>
       </c>
@@ -3843,7 +4273,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6">
       <c r="A101" s="1" t="s">
         <v>294</v>
       </c>
@@ -3860,7 +4290,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6">
       <c r="A102" s="1" t="s">
         <v>297</v>
       </c>
@@ -3877,7 +4307,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6">
       <c r="A103" s="1" t="s">
         <v>300</v>
       </c>
@@ -3894,7 +4324,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6">
       <c r="A104" s="1" t="s">
         <v>303</v>
       </c>
@@ -3911,7 +4341,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6">
       <c r="A105" s="1" t="s">
         <v>306</v>
       </c>
@@ -3928,7 +4358,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6">
       <c r="A106" s="1" t="s">
         <v>309</v>
       </c>
@@ -3945,7 +4375,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6">
       <c r="A107" s="1" t="s">
         <v>312</v>
       </c>
@@ -3962,7 +4392,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6">
       <c r="A108" s="1" t="s">
         <v>315</v>
       </c>
@@ -3979,7 +4409,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6">
       <c r="A109" s="1" t="s">
         <v>318</v>
       </c>
@@ -3996,7 +4426,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6">
       <c r="A110" s="1" t="s">
         <v>321</v>
       </c>
@@ -4013,7 +4443,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6">
       <c r="A111" s="1" t="s">
         <v>324</v>
       </c>
@@ -4030,7 +4460,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6">
       <c r="A112" s="1" t="s">
         <v>327</v>
       </c>
@@ -4047,7 +4477,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6">
       <c r="A113" s="1" t="s">
         <v>330</v>
       </c>
@@ -4064,7 +4494,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6">
       <c r="A114" s="1" t="s">
         <v>333</v>
       </c>
@@ -4081,7 +4511,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6">
       <c r="A115" s="1" t="s">
         <v>336</v>
       </c>
@@ -4098,7 +4528,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6">
       <c r="A116" s="1" t="s">
         <v>340</v>
       </c>
@@ -4115,7 +4545,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6">
       <c r="A117" s="1" t="s">
         <v>343</v>
       </c>
@@ -4132,7 +4562,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6">
       <c r="A118" s="1" t="s">
         <v>346</v>
       </c>
@@ -4149,7 +4579,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6">
       <c r="A119" s="1" t="s">
         <v>349</v>
       </c>
@@ -4166,7 +4596,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6">
       <c r="A120" s="1" t="s">
         <v>352</v>
       </c>
@@ -4183,7 +4613,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6">
       <c r="A121" s="1" t="s">
         <v>355</v>
       </c>
@@ -4200,7 +4630,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6">
       <c r="A122" s="1" t="s">
         <v>358</v>
       </c>
@@ -4217,7 +4647,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6">
       <c r="A123" s="1" t="s">
         <v>361</v>
       </c>
@@ -4234,7 +4664,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6">
       <c r="A124" s="1" t="s">
         <v>364</v>
       </c>
@@ -4251,7 +4681,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6">
       <c r="A125" s="1" t="s">
         <v>367</v>
       </c>
@@ -4268,7 +4698,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6">
       <c r="A126" s="1" t="s">
         <v>370</v>
       </c>
@@ -4285,7 +4715,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6">
       <c r="A127" s="1" t="s">
         <v>373</v>
       </c>
@@ -4302,7 +4732,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6">
       <c r="A128" s="1" t="s">
         <v>376</v>
       </c>
@@ -4319,7 +4749,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6">
       <c r="A129" s="1" t="s">
         <v>379</v>
       </c>
@@ -4336,7 +4766,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6">
       <c r="A130" s="1" t="s">
         <v>383</v>
       </c>
@@ -4353,7 +4783,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6">
       <c r="A131" s="1" t="s">
         <v>385</v>
       </c>
@@ -4370,7 +4800,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6">
       <c r="A132" s="1" t="s">
         <v>388</v>
       </c>
@@ -4387,7 +4817,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6">
       <c r="A133" s="1" t="s">
         <v>392</v>
       </c>
@@ -4404,7 +4834,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6">
       <c r="A134" s="1" t="s">
         <v>395</v>
       </c>
@@ -4421,7 +4851,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6">
       <c r="A135" s="1" t="s">
         <v>398</v>
       </c>
@@ -4438,7 +4868,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6">
       <c r="A136" s="1" t="s">
         <v>539</v>
       </c>
@@ -4455,7 +4885,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6">
       <c r="A137" s="1" t="s">
         <v>401</v>
       </c>
@@ -4472,7 +4902,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6">
       <c r="A138" s="1" t="s">
         <v>403</v>
       </c>
@@ -4489,7 +4919,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6">
       <c r="A139" s="1" t="s">
         <v>406</v>
       </c>
@@ -4506,7 +4936,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6">
       <c r="A140" s="1" t="s">
         <v>536</v>
       </c>
@@ -4523,7 +4953,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6">
       <c r="A141" s="1" t="s">
         <v>409</v>
       </c>
@@ -4540,7 +4970,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6">
       <c r="A142" s="1" t="s">
         <v>412</v>
       </c>
@@ -4557,7 +4987,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6">
       <c r="A143" s="1" t="s">
         <v>414</v>
       </c>
@@ -4574,7 +5004,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6">
       <c r="A144" s="1" t="s">
         <v>417</v>
       </c>
@@ -4591,7 +5021,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6">
       <c r="A145" s="1" t="s">
         <v>419</v>
       </c>
@@ -4608,7 +5038,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6">
       <c r="A146" s="1" t="s">
         <v>422</v>
       </c>
@@ -4625,7 +5055,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6">
       <c r="A147" s="1" t="s">
         <v>424</v>
       </c>
@@ -4642,7 +5072,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6">
       <c r="A148" s="1" t="s">
         <v>427</v>
       </c>
@@ -4659,7 +5089,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6">
       <c r="A149" s="1" t="s">
         <v>429</v>
       </c>
@@ -4676,7 +5106,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6">
       <c r="A150" s="1" t="s">
         <v>432</v>
       </c>
@@ -4691,10 +5121,2068 @@
       </c>
       <c r="F150" s="1" t="s">
         <v>526</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>568</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166EE81A-B3F4-47DE-9841-E72857BFDC81}">
+  <dimension ref="A1:C157"/>
+  <sheetViews>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C1" t="str" cm="1">
+        <f t="array" ref="C1">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A1,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C2" t="str" cm="1">
+        <f t="array" ref="C2">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A2,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C3" t="str" cm="1">
+        <f t="array" ref="C3">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A3,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" t="str" cm="1">
+        <f t="array" ref="C4">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A4,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C5" t="str" cm="1">
+        <f t="array" ref="C5">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A5,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C6" t="str" cm="1">
+        <f t="array" ref="C6">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A6,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C7" t="str" cm="1">
+        <f t="array" ref="C7">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A7,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C8" t="str" cm="1">
+        <f t="array" ref="C8">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A8,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C9" t="str" cm="1">
+        <f t="array" ref="C9">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A9,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C10" t="str" cm="1">
+        <f t="array" ref="C10">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A10,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C11" t="str" cm="1">
+        <f t="array" ref="C11">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A11,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C12" t="str" cm="1">
+        <f t="array" ref="C12">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A12,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C13" t="str" cm="1">
+        <f t="array" ref="C13">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A13,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C14" t="str" cm="1">
+        <f t="array" ref="C14">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A14,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C15" t="str" cm="1">
+        <f t="array" ref="C15">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A15,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C16" t="str" cm="1">
+        <f t="array" ref="C16">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A16,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C17" t="str" cm="1">
+        <f t="array" ref="C17">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A17,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C18" t="str" cm="1">
+        <f t="array" ref="C18">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A18,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C19" t="str" cm="1">
+        <f t="array" ref="C19">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A19,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C20" t="str" cm="1">
+        <f t="array" ref="C20">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A20,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C21" t="str" cm="1">
+        <f t="array" ref="C21">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A21,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="C22" t="str" cm="1">
+        <f t="array" ref="C22">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A22,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C23" t="str" cm="1">
+        <f t="array" ref="C23">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A23,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C24" t="str" cm="1">
+        <f t="array" ref="C24">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A24,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C25" t="str" cm="1">
+        <f t="array" ref="C25">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A25,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C26" t="str" cm="1">
+        <f t="array" ref="C26">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A26,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C27" t="str" cm="1">
+        <f t="array" ref="C27">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A27,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C28" t="str" cm="1">
+        <f t="array" ref="C28">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A28,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C29" t="str" cm="1">
+        <f t="array" ref="C29">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A29,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C30" t="str" cm="1">
+        <f t="array" ref="C30">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A30,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C31" t="str" cm="1">
+        <f t="array" ref="C31">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A31,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C32" t="str" cm="1">
+        <f t="array" ref="C32">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A32,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C33" t="str" cm="1">
+        <f t="array" ref="C33">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A33,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C34" t="str" cm="1">
+        <f t="array" ref="C34">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A34,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C35" t="str" cm="1">
+        <f t="array" ref="C35">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A35,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C36" t="str" cm="1">
+        <f t="array" ref="C36">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A36,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C37" t="str" cm="1">
+        <f t="array" ref="C37">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A37,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C38" t="str" cm="1">
+        <f t="array" ref="C38">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A38,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C39" t="str" cm="1">
+        <f t="array" ref="C39">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A39,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C40" t="str" cm="1">
+        <f t="array" ref="C40">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A40,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C41" t="str" cm="1">
+        <f t="array" ref="C41">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A41,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C42" t="str" cm="1">
+        <f t="array" ref="C42">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A42,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C43" t="str" cm="1">
+        <f t="array" ref="C43">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A43,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C44" t="str" cm="1">
+        <f t="array" ref="C44">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A44,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C45" t="str" cm="1">
+        <f t="array" ref="C45">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A45,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C46" t="str" cm="1">
+        <f t="array" ref="C46">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A46,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C47" t="str" cm="1">
+        <f t="array" ref="C47">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A47,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C48" t="str" cm="1">
+        <f t="array" ref="C48">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A48,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C49" t="str" cm="1">
+        <f t="array" ref="C49">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A49,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C50" t="str" cm="1">
+        <f t="array" ref="C50">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A50,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C51" t="str" cm="1">
+        <f t="array" ref="C51">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A51,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C52" t="str" cm="1">
+        <f t="array" ref="C52">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A52,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C53" t="str" cm="1">
+        <f t="array" ref="C53">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A53,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C54" t="str" cm="1">
+        <f t="array" ref="C54">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A54,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C55" t="str" cm="1">
+        <f t="array" ref="C55">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A55,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C56" t="str" cm="1">
+        <f t="array" ref="C56">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A56,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C57" t="str" cm="1">
+        <f t="array" ref="C57">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A57,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C58" t="str" cm="1">
+        <f t="array" ref="C58">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A58,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C59" t="str" cm="1">
+        <f t="array" ref="C59">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A59,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C60" t="str" cm="1">
+        <f t="array" ref="C60">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A60,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C61" t="str" cm="1">
+        <f t="array" ref="C61">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A61,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C62" t="str" cm="1">
+        <f t="array" ref="C62">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A62,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C63" t="str" cm="1">
+        <f t="array" ref="C63">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A63,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C64" t="str" cm="1">
+        <f t="array" ref="C64">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A64,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C65" t="str" cm="1">
+        <f t="array" ref="C65">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A65,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C66" t="str" cm="1">
+        <f t="array" ref="C66">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A66,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C67" t="str" cm="1">
+        <f t="array" ref="C67">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A67,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C68" t="str" cm="1">
+        <f t="array" ref="C68">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A68,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C69" t="str" cm="1">
+        <f t="array" ref="C69">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A69,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C70" t="str" cm="1">
+        <f t="array" ref="C70">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A70,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C71" t="str" cm="1">
+        <f t="array" ref="C71">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A71,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C72" t="str" cm="1">
+        <f t="array" ref="C72">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A72,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C73" t="str" cm="1">
+        <f t="array" ref="C73">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A73,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C74" t="str" cm="1">
+        <f t="array" ref="C74">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A74,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C75" t="str" cm="1">
+        <f t="array" ref="C75">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A75,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C76" t="str" cm="1">
+        <f t="array" ref="C76">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A76,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C77" t="str" cm="1">
+        <f t="array" ref="C77">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A77,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="C78" t="str" cm="1">
+        <f t="array" ref="C78">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A78,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="C79" t="str" cm="1">
+        <f t="array" ref="C79">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A79,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C80" t="str" cm="1">
+        <f t="array" ref="C80">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A80,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C81" t="str" cm="1">
+        <f t="array" ref="C81">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A81,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C82" t="str" cm="1">
+        <f t="array" ref="C82">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A82,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C83" t="str" cm="1">
+        <f t="array" ref="C83">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A83,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C84" t="str" cm="1">
+        <f t="array" ref="C84">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A84,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C85" t="str" cm="1">
+        <f t="array" ref="C85">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A85,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C86" t="str" cm="1">
+        <f t="array" ref="C86">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A86,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C87" t="str" cm="1">
+        <f t="array" ref="C87">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A87,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="C88" t="str" cm="1">
+        <f t="array" ref="C88">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A88,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C89" t="str" cm="1">
+        <f t="array" ref="C89">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A89,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C90" t="str" cm="1">
+        <f t="array" ref="C90">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A90,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C91" t="str" cm="1">
+        <f t="array" ref="C91">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A91,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C92" t="str" cm="1">
+        <f t="array" ref="C92">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A92,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C93" t="str" cm="1">
+        <f t="array" ref="C93">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A93,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C94" t="str" cm="1">
+        <f t="array" ref="C94">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A94,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C95" t="str" cm="1">
+        <f t="array" ref="C95">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A95,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C96" t="str" cm="1">
+        <f t="array" ref="C96">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A96,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C97" t="str" cm="1">
+        <f t="array" ref="C97">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A97,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="C98" t="str" cm="1">
+        <f t="array" ref="C98">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A98,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C99" t="str" cm="1">
+        <f t="array" ref="C99">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A99,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C100" t="str" cm="1">
+        <f t="array" ref="C100">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A100,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="C101" t="str" cm="1">
+        <f t="array" ref="C101">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A101,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C102" t="str" cm="1">
+        <f t="array" ref="C102">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A102,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="C103" t="str" cm="1">
+        <f t="array" ref="C103">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A103,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C104" t="str" cm="1">
+        <f t="array" ref="C104">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A104,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C105" t="str" cm="1">
+        <f t="array" ref="C105">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A105,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C106" t="str" cm="1">
+        <f t="array" ref="C106">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A106,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C107" t="str" cm="1">
+        <f t="array" ref="C107">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A107,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="C108" t="str" cm="1">
+        <f t="array" ref="C108">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A108,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C109" t="str" cm="1">
+        <f t="array" ref="C109">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A109,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C110" t="str" cm="1">
+        <f t="array" ref="C110">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A110,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C111" t="str" cm="1">
+        <f t="array" ref="C111">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A111,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="C112" t="str" cm="1">
+        <f t="array" ref="C112">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A112,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C113" t="str" cm="1">
+        <f t="array" ref="C113">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A113,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C114" t="str" cm="1">
+        <f t="array" ref="C114">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A114,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C115" t="str" cm="1">
+        <f t="array" ref="C115">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A115,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C116" t="str" cm="1">
+        <f t="array" ref="C116">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A116,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="C117" t="str" cm="1">
+        <f t="array" ref="C117">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A117,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C118" t="str" cm="1">
+        <f t="array" ref="C118">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A118,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C119" t="str" cm="1">
+        <f t="array" ref="C119">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A119,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="C120" t="str" cm="1">
+        <f t="array" ref="C120">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A120,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C121" t="str" cm="1">
+        <f t="array" ref="C121">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A121,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C122" t="str" cm="1">
+        <f t="array" ref="C122">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A122,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C123" t="str" cm="1">
+        <f t="array" ref="C123">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A123,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C124" t="str" cm="1">
+        <f t="array" ref="C124">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A124,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C125" t="str" cm="1">
+        <f t="array" ref="C125">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A125,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="C126" t="str" cm="1">
+        <f t="array" ref="C126">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A126,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C127" t="str" cm="1">
+        <f t="array" ref="C127">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A127,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C128" t="str" cm="1">
+        <f t="array" ref="C128">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A128,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="C129" t="str" cm="1">
+        <f t="array" ref="C129">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A129,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="C130" t="str" cm="1">
+        <f t="array" ref="C130">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A130,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C131" t="str" cm="1">
+        <f t="array" ref="C131">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A131,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C132" t="str" cm="1">
+        <f t="array" ref="C132">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A132,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C133" t="str" cm="1">
+        <f t="array" ref="C133">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A133,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="C134" t="str" cm="1">
+        <f t="array" ref="C134">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A134,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C135" t="str" cm="1">
+        <f t="array" ref="C135">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A135,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="C136" t="str" cm="1">
+        <f t="array" ref="C136">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A136,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C137" t="str" cm="1">
+        <f t="array" ref="C137">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A137,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C138" t="str" cm="1">
+        <f t="array" ref="C138">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A138,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C139" t="str" cm="1">
+        <f t="array" ref="C139">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A139,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="C140" t="str" cm="1">
+        <f t="array" ref="C140">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A140,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="C141" t="str" cm="1">
+        <f t="array" ref="C141">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A141,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C142" t="str" cm="1">
+        <f t="array" ref="C142">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A142,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C143" t="str" cm="1">
+        <f t="array" ref="C143">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A143,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="C144" t="str" cm="1">
+        <f t="array" ref="C144">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A144,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="C145" t="str" cm="1">
+        <f t="array" ref="C145">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A145,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C146" t="str" cm="1">
+        <f t="array" ref="C146">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A146,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C147" t="str" cm="1">
+        <f t="array" ref="C147">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A147,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="C148" t="str" cm="1">
+        <f t="array" ref="C148">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A148,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="C149" t="str" cm="1">
+        <f t="array" ref="C149">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A149,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C150" t="str" cm="1">
+        <f t="array" ref="C150">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A150,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="C151" t="str" cm="1">
+        <f t="array" ref="C151">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A151,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C152" t="str" cm="1">
+        <f t="array" ref="C152">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A152,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C153" t="str" cm="1">
+        <f t="array" ref="C153">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A153,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C154" t="str" cm="1">
+        <f t="array" ref="C154">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A154,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="C155" t="str" cm="1">
+        <f t="array" ref="C155">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A155,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C156" t="str" cm="1">
+        <f t="array" ref="C156">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A156,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="C157" t="str" cm="1">
+        <f t="array" ref="C157">_xlfn.LAMBDA(_xlpm.x,IF(ISERROR(_xlpm.x),"NODE NOT FOUND",""))(VLOOKUP(A157,Main_240213!$A$2:$A$8004,1,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>